<commit_message>
Update: forecast, and Inflation rate
</commit_message>
<xml_diff>
--- a/Dolar_Today.xlsx
+++ b/Dolar_Today.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\OneDrive\DS_Projects\Exchange_Rate_Venezuela\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\OneDrive\DS_Projects\Exchange_Rate_Venezuela\exchange_rate_Venezuela\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09F9F8C-6B58-47A7-AAC6-D622D359924C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22553F7B-7224-49EC-9DE1-859E55D1A05A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3233" uniqueCount="3233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3246" uniqueCount="3246">
   <si>
     <t>Fecha</t>
   </si>
@@ -9730,6 +9730,45 @@
   </si>
   <si>
     <t>10-10-2019</t>
+  </si>
+  <si>
+    <t>10-11-2019</t>
+  </si>
+  <si>
+    <t>10-12-2019</t>
+  </si>
+  <si>
+    <t>10-13-2019</t>
+  </si>
+  <si>
+    <t>10-14-2019</t>
+  </si>
+  <si>
+    <t>10-15-2019</t>
+  </si>
+  <si>
+    <t>10-16-2019</t>
+  </si>
+  <si>
+    <t>10-17-2019</t>
+  </si>
+  <si>
+    <t>10-18-2019</t>
+  </si>
+  <si>
+    <t>10-19-2019</t>
+  </si>
+  <si>
+    <t>10-20-2019</t>
+  </si>
+  <si>
+    <t>10-21-2019</t>
+  </si>
+  <si>
+    <t>10-22-2019</t>
+  </si>
+  <si>
+    <t>10-23-2019</t>
   </si>
 </sst>
 </file>
@@ -9790,7 +9829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -9800,6 +9839,7 @@
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -10115,10 +10155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3232"/>
+  <dimension ref="A1:B3245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3212" workbookViewId="0">
-      <selection activeCell="A3226" sqref="A3226"/>
+    <sheetView tabSelected="1" topLeftCell="A3227" workbookViewId="0">
+      <selection activeCell="B3234" sqref="B3234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35983,6 +36023,110 @@
         <v>1986106000.0000002</v>
       </c>
     </row>
+    <row r="3233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3233" s="2" t="s">
+        <v>3233</v>
+      </c>
+      <c r="B3233" s="4">
+        <v>1993204000</v>
+      </c>
+    </row>
+    <row r="3234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3234" s="2" t="s">
+        <v>3234</v>
+      </c>
+      <c r="B3234" s="4">
+        <v>1993204000</v>
+      </c>
+    </row>
+    <row r="3235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3235" s="2" t="s">
+        <v>3235</v>
+      </c>
+      <c r="B3235" s="4">
+        <v>1993204000</v>
+      </c>
+    </row>
+    <row r="3236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3236" s="2" t="s">
+        <v>3236</v>
+      </c>
+      <c r="B3236" s="4">
+        <v>1963541000</v>
+      </c>
+    </row>
+    <row r="3237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3237" s="2" t="s">
+        <v>3237</v>
+      </c>
+      <c r="B3237" s="4">
+        <v>1950221000</v>
+      </c>
+    </row>
+    <row r="3238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3238" s="2" t="s">
+        <v>3238</v>
+      </c>
+      <c r="B3238" s="4">
+        <v>1919906000.0000002</v>
+      </c>
+    </row>
+    <row r="3239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3239" s="5" t="s">
+        <v>3239</v>
+      </c>
+      <c r="B3239" s="4">
+        <v>1919906000.0000002</v>
+      </c>
+    </row>
+    <row r="3240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3240" s="5" t="s">
+        <v>3240</v>
+      </c>
+      <c r="B3240" s="4">
+        <v>1903249000.0000002</v>
+      </c>
+    </row>
+    <row r="3241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3241" s="5" t="s">
+        <v>3241</v>
+      </c>
+      <c r="B3241" s="4">
+        <v>1903249000.0000002</v>
+      </c>
+    </row>
+    <row r="3242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3242" s="5" t="s">
+        <v>3242</v>
+      </c>
+      <c r="B3242" s="4">
+        <v>1903249000.0000002</v>
+      </c>
+    </row>
+    <row r="3243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3243" s="5" t="s">
+        <v>3243</v>
+      </c>
+      <c r="B3243" s="4">
+        <v>1870402000</v>
+      </c>
+    </row>
+    <row r="3244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3244" s="5" t="s">
+        <v>3244</v>
+      </c>
+      <c r="B3244" s="4">
+        <v>1850264000</v>
+      </c>
+    </row>
+    <row r="3245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3245" s="5" t="s">
+        <v>3245</v>
+      </c>
+      <c r="B3245" s="4">
+        <v>1883020000</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>